<commit_message>
Update Germplasm sample files with "Germplasm Name" as column name.
</commit_message>
<xml_diff>
--- a/src/files/GermplasmImport/Germplasm77_2022-07-12 - Copy.xlsx
+++ b/src/files/GermplasmImport/Germplasm77_2022-07-12 - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tep46/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\breedinginsight\cucumber\src\files\GermplasmImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42194985-BD35-DB42-9235-1C52759F8488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057F0EEE-3D9F-4FC6-A997-808A6EC3740B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-12" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Germplasm Import" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>GID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Breeding Method</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Male complex top cross</t>
+  </si>
+  <si>
+    <t>Germplasm Name</t>
   </si>
 </sst>
 </file>
@@ -482,88 +482,88 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -575,21 +575,21 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -601,21 +601,21 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -627,47 +627,47 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
       <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -679,47 +679,47 @@
         <v>3</v>
       </c>
       <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>7</v>
       </c>
       <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -731,47 +731,47 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
       <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
         <v>14</v>
       </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -783,10 +783,10 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>